<commit_message>
neu Harkenblecker und B3alt
</commit_message>
<xml_diff>
--- a/MaengelKarte/Maengelliste.xlsx
+++ b/MaengelKarte/Maengelliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataADFC\1_ADFC-github\adfc-hemmingen-pattensen.github.io\MaengelKarte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927EECDC-AAA9-451E-9F2A-113E2AC0C6AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F5D574-A478-4ECF-90AA-DE1C2150EE13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="937">
   <si>
     <t>ADFC Hemmingen / Pattensen</t>
   </si>
@@ -3124,6 +3124,43 @@
     <t>- offen
 - 2020 - Innerhin stehen im Haushaltsplan für 2020 ca. 10000 €uro für die Unterhaltung der Wirtschafts- und Wanderwege (Für Material und Einsatz des Wegehobels).
 - 2021-01 Kontakt mit Ralf Mannstedt aud Linderte - Dort nennt man diese Maßnahme "M1"</t>
+  </si>
+  <si>
+    <t>7PXW+85</t>
+  </si>
+  <si>
+    <t>per Email</t>
+  </si>
+  <si>
+    <t>Harkenblecker Weg in Arnum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Situation als Radfahrerin ist dort aktuell ziemlich unglücklich. Offiziell gehören Radfahrer*innen auf die Straße. Das ist natürlich auch nicht anders möglich, denn die Seitenanlagen sind beidseits so schmal, dass man, besonders mit Lastenrad oder Kinderanhänger, kaum an entgegenkommenden Fußgänger*innen vorbei kommt.
+Trotzdem fahren die meisten Radfahrer*innen auf dem reinen Fußweg, denn auf der Straße fühlt man sich, besonders mit Kind im Anhänger, in einer Tempo 50 Zone wirklich nicht wohl.
+Bis auf ein Verkehrsschild „Achtung Radfahrer“ (138-10) kurz nach dem Ortseingang (da parkt oft ein LKW, weshalb die Autofahrer das Schild nicht einmal sehen), weist nichts darauf hin, dass Radfahrer hier rechtmäßig auf die Straße gehören. </t>
+  </si>
+  <si>
+    <t>Auf der Straße fühlt man sich nicht wohl</t>
+  </si>
+  <si>
+    <t>Eventuell Fahrrad-Symbole auf der Fahrbahn (wie in der Ortsdurchfahrt Jeinsen oder Devese) oder eine kombinierte Lösung mit Schutzstreifen auf einer Seite (wie in Pattensen, Jeinser Straße). Zusätzliche Möglichkeit der Tempo-Reduzierung.</t>
+  </si>
+  <si>
+    <t>8PCG+CM</t>
+  </si>
+  <si>
+    <t>Kfz dürfen nicht Überholen</t>
+  </si>
+  <si>
+    <t>Göttinger Landstraße - zwischen Kirchdamm und Weetzener Landstr.</t>
+  </si>
+  <si>
+    <t>Die Umbaupläne sehen zwischen den nicht befahrbaren Gleisbett und dem Hochboard eine 3 m breite Fahrbahn und einen 1,5 m breiten Schutzstreifen, in beiden Richtungen, vor. Für den Radfahrenden bleiben ca. 1,2 m wegen der Regenrinne zum fahren. Wenn hier ein Radfahrer:innen unterwegs ist, bleibt noch die Fahrbahnbreite von 3m übrig zum Überholen. Das reicht nicht, um den Sicherheitsabstand einzuhalten, und das über eine Länge von 800 m. Es sei denn das Kfz ist schmaler als 1,5 m.</t>
+  </si>
+  <si>
+    <t>1. Radfahrende auf einen seperaten Radweg führen.
+2. Überholverbot verdeutlichen mit 
+![](8PCG+CM_Stadtbahnverlängerung2.svg)</t>
   </si>
 </sst>
 </file>
@@ -3358,7 +3395,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3480,12 +3517,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3877,9 +3908,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ275"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H257" sqref="H257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4318,7 +4349,7 @@
       <c r="H10" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="52" t="s">
         <v>925</v>
       </c>
       <c r="J10" s="27"/>
@@ -14166,7 +14197,7 @@
       <c r="H177" s="26" t="s">
         <v>704</v>
       </c>
-      <c r="I177" s="54" t="s">
+      <c r="I177" s="52" t="s">
         <v>924</v>
       </c>
       <c r="J177" s="27"/>
@@ -15313,7 +15344,7 @@
         <v>811</v>
       </c>
       <c r="B199" s="22" t="str">
-        <f t="shared" ref="B199:B254" si="19">HYPERLINK(CONCATENATE("https://www.google.com/maps/search/?api=1&amp;query=9F4F",LEFT(A199,4),"%2B",RIGHT(A199,2)),A199)</f>
+        <f t="shared" ref="B199:B256" si="19">HYPERLINK(CONCATENATE("https://www.google.com/maps/search/?api=1&amp;query=9F4F",LEFT(A199,4),"%2B",RIGHT(A199,2)),A199)</f>
         <v>Gute Radwege</v>
       </c>
       <c r="C199" s="37"/>
@@ -18037,12 +18068,102 @@
       <c r="Z254" s="32"/>
       <c r="AA254" s="32"/>
     </row>
-    <row r="255" spans="1:27" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B255" s="2"/>
-      <c r="I255" s="52"/>
-      <c r="J255" s="53"/>
-    </row>
-    <row r="256" spans="1:27" ht="85.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" spans="1:27" ht="133.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A255" s="39" t="s">
+        <v>926</v>
+      </c>
+      <c r="B255" s="22" t="str">
+        <f t="shared" si="19"/>
+        <v>7PXW+85</v>
+      </c>
+      <c r="C255" s="40" t="s">
+        <v>930</v>
+      </c>
+      <c r="D255" s="41">
+        <v>44318</v>
+      </c>
+      <c r="E255" s="41" t="s">
+        <v>927</v>
+      </c>
+      <c r="F255" s="40" t="s">
+        <v>928</v>
+      </c>
+      <c r="G255" s="40" t="s">
+        <v>929</v>
+      </c>
+      <c r="H255" s="26" t="s">
+        <v>931</v>
+      </c>
+      <c r="I255" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="J255" s="27"/>
+      <c r="K255" s="29"/>
+      <c r="L255" s="29"/>
+      <c r="M255" s="42"/>
+      <c r="N255" s="43"/>
+      <c r="O255" s="32"/>
+      <c r="P255" s="32"/>
+      <c r="Q255" s="32"/>
+      <c r="R255" s="32"/>
+      <c r="S255" s="32"/>
+      <c r="T255" s="32"/>
+      <c r="U255" s="32"/>
+      <c r="V255" s="32"/>
+      <c r="W255" s="32"/>
+      <c r="X255" s="32"/>
+      <c r="Y255" s="32"/>
+      <c r="Z255" s="32"/>
+      <c r="AA255" s="32"/>
+    </row>
+    <row r="256" spans="1:27" ht="133.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="39" t="s">
+        <v>932</v>
+      </c>
+      <c r="B256" s="22" t="str">
+        <f t="shared" si="19"/>
+        <v>8PCG+CM</v>
+      </c>
+      <c r="C256" s="40" t="s">
+        <v>933</v>
+      </c>
+      <c r="D256" s="41">
+        <v>44318</v>
+      </c>
+      <c r="E256" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F256" s="40" t="s">
+        <v>934</v>
+      </c>
+      <c r="G256" s="40" t="s">
+        <v>935</v>
+      </c>
+      <c r="H256" s="26" t="s">
+        <v>936</v>
+      </c>
+      <c r="I256" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="J256" s="27"/>
+      <c r="K256" s="29"/>
+      <c r="L256" s="29"/>
+      <c r="M256" s="42"/>
+      <c r="N256" s="43"/>
+      <c r="O256" s="32"/>
+      <c r="P256" s="32"/>
+      <c r="Q256" s="32"/>
+      <c r="R256" s="32"/>
+      <c r="S256" s="32"/>
+      <c r="T256" s="32"/>
+      <c r="U256" s="32"/>
+      <c r="V256" s="32"/>
+      <c r="W256" s="32"/>
+      <c r="X256" s="32"/>
+      <c r="Y256" s="32"/>
+      <c r="Z256" s="32"/>
+      <c r="AA256" s="32"/>
+    </row>
     <row r="257" ht="85.15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="258" ht="85.15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="259" ht="85.15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
lin maengel on top
</commit_message>
<xml_diff>
--- a/MaengelKarte/Maengelliste.xlsx
+++ b/MaengelKarte/Maengelliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataADFC\1_ADFC-github\adfc-hemmingen-pattensen.github.io\MaengelKarte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5873A670-416C-4A19-B6AA-4131EF6CC13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F10DAC-1965-4617-AB38-35F2B9EDD8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="1003">
   <si>
     <t>ADFC Hemmingen / Pattensen</t>
   </si>
@@ -3359,6 +3359,21 @@
   </si>
   <si>
     <t>8PFJ+PH</t>
+  </si>
+  <si>
+    <t>Durchfahrtverbot für alle, auch Fahrräder.</t>
+  </si>
+  <si>
+    <t>Radfahrer frei fehlt</t>
+  </si>
+  <si>
+    <t>Radfahrer frei anbringen</t>
+  </si>
+  <si>
+    <t>8PJR+26</t>
+  </si>
+  <si>
+    <t>wurde asphaltiert</t>
   </si>
 </sst>
 </file>
@@ -4124,8 +4139,8 @@
   <dimension ref="A1:AMJ277"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C267" sqref="C267"/>
+      <pane ySplit="6" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I144" sqref="I144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -12501,9 +12516,11 @@
         <v>622</v>
       </c>
       <c r="I144" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="J144" s="27"/>
+        <v>1002</v>
+      </c>
+      <c r="J144" s="27" t="s">
+        <v>43</v>
+      </c>
       <c r="K144" s="28" t="str">
         <f t="shared" si="13"/>
         <v>8PJR+46</v>
@@ -12559,9 +12576,11 @@
         <v>622</v>
       </c>
       <c r="I145" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="J145" s="27"/>
+        <v>1002</v>
+      </c>
+      <c r="J145" s="27" t="s">
+        <v>43</v>
+      </c>
       <c r="K145" s="28" t="str">
         <f t="shared" si="13"/>
         <v>8PJR+46</v>
@@ -18965,7 +18984,59 @@
       <c r="Z266" s="55"/>
       <c r="AA266" s="55"/>
     </row>
-    <row r="267" spans="1:27" ht="85.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" spans="1:27" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A267" s="39" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B267" s="56" t="str">
+        <f t="shared" ref="B267" si="32">HYPERLINK(CONCATENATE("https://www.google.com/maps/search/?api=1&amp;query=9F4F",LEFT(A267,4),"%2B",RIGHT(A267,2)),A267)</f>
+        <v>8PJR+26</v>
+      </c>
+      <c r="C267" s="40" t="s">
+        <v>998</v>
+      </c>
+      <c r="D267" s="41">
+        <v>44748</v>
+      </c>
+      <c r="E267" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F267" s="40" t="s">
+        <v>624</v>
+      </c>
+      <c r="G267" s="40" t="s">
+        <v>999</v>
+      </c>
+      <c r="H267" s="40" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I267" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J267" s="52"/>
+      <c r="K267" s="28" t="str">
+        <f t="shared" ref="K267" si="33">HYPERLINK(CONCATENATE("https://plus.codes/9F4F",A267),A267)</f>
+        <v>8PJR+26</v>
+      </c>
+      <c r="L267" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="M267" s="53"/>
+      <c r="N267" s="54"/>
+      <c r="O267" s="55"/>
+      <c r="P267" s="55"/>
+      <c r="Q267" s="55"/>
+      <c r="R267" s="55"/>
+      <c r="S267" s="55"/>
+      <c r="T267" s="55"/>
+      <c r="U267" s="55"/>
+      <c r="V267" s="55"/>
+      <c r="W267" s="55"/>
+      <c r="X267" s="55"/>
+      <c r="Y267" s="55"/>
+      <c r="Z267" s="55"/>
+      <c r="AA267" s="55"/>
+    </row>
     <row r="268" spans="1:27" ht="85.15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="269" spans="1:27" ht="85.15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="270" spans="1:27" ht="85.15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>